<commit_message>
Generics and Collections. task 04 has been completed
</commit_message>
<xml_diff>
--- a/src/_java/_se/_06/_task01/table collections.xlsx
+++ b/src/_java/_se/_06/_task01/table collections.xlsx
@@ -231,603 +231,627 @@
     <t>Blocking Operations</t>
   </si>
   <si>
-    <t>public class LinkedList&lt;E&gt;
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ConcurrentLinkedDeque&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractCollection&lt;E&gt;
+implements Deque&lt;E&gt;, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>public class</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ArrayBlockingQueue&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractQueue&lt;E&gt;
+implements BlockingQueue&lt;E&gt;, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>public class</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CopyOnWriteArrayList&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends Object
+implements List&lt;E&gt;, RandomAccess, Cloneable, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DelayQueue&lt;E extends Delayed&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractQueue&lt;E&gt;
+implements BlockingQueue&lt;E&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LinkedBlockingDeque&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractQueue&lt;E&gt;
+implements BlockingDeque&lt;E&gt;, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LinkedBlockingQueue&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractQueue&lt;E&gt;
+implements BlockingQueue&lt;E&gt;, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LinkedTransferQueue&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractQueue&lt;E&gt;
+implements TransferQueue&lt;E&gt;, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PriorityBlockingQueue&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractQueue&lt;E&gt;
+implements BlockingQueue&lt;E&gt;, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>public class</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> PriorityQueue&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractQueue&lt;E&gt;
+implements Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Stack&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends Vector&lt;E&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SynchronousQueue&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractQueue&lt;E&gt;
+implements BlockingQueue&lt;E&gt;, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>public class</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vector&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractList&lt;E&gt;
+implements List&lt;E&gt;, RandomAccess, Cloneable, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>public class</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TreeSet&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractSet&lt;E&gt;
+implements NavigableSet&lt;E&gt;, Cloneable, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LinkedHashSet&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends HashSet&lt;E&gt;
+implements Set&lt;E&gt;, Cloneable, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <t>The Collections Framework</t>
+  </si>
+  <si>
+    <t>FIFO (first-in-first-out)</t>
+  </si>
+  <si>
+    <t>Interface Collection&lt;E&gt;</t>
+  </si>
+  <si>
+    <t>Interface Map&lt;K,V&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ArrayDeque&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractCollection&lt;E&gt;
+implements Deque&lt;E&gt;, Cloneable, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ArrayList&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractList&lt;E&gt;
+implements List&lt;E&gt;, RandomAccess, Cloneable, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ConcurrentLinkedQueue&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractQueue&lt;E&gt;
+implements Queue&lt;E&gt;, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ConcurrentSkipListSet&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractSet&lt;E&gt;
+implements NavigableSet&lt;E&gt;, Cloneable, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>public class</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CopyOnWriteArraySet&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractSet&lt;E&gt;
+implements Serializable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HashSet&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extends AbstractSet&lt;E&gt;
+implements Set&lt;E&gt;, Cloneable, Serializable</t>
+    </r>
+  </si>
+  <si>
+    <t> last-in-first-out (LIFO) </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LinkedList&lt;E&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 extends AbstractSequentialList&lt;E&gt;
 implements List&lt;E&gt;, Deque&lt;E&gt;, Cloneable, Serializable</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ConcurrentLinkedDeque&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractCollection&lt;E&gt;
-implements Deque&lt;E&gt;, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>public class</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ArrayBlockingQueue&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractQueue&lt;E&gt;
-implements BlockingQueue&lt;E&gt;, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>public class</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CopyOnWriteArrayList&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends Object
-implements List&lt;E&gt;, RandomAccess, Cloneable, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DelayQueue&lt;E extends Delayed&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractQueue&lt;E&gt;
-implements BlockingQueue&lt;E&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LinkedBlockingDeque&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractQueue&lt;E&gt;
-implements BlockingDeque&lt;E&gt;, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LinkedBlockingQueue&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractQueue&lt;E&gt;
-implements BlockingQueue&lt;E&gt;, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LinkedTransferQueue&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractQueue&lt;E&gt;
-implements TransferQueue&lt;E&gt;, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PriorityBlockingQueue&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractQueue&lt;E&gt;
-implements BlockingQueue&lt;E&gt;, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>public class</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> PriorityQueue&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractQueue&lt;E&gt;
-implements Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Stack&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends Vector&lt;E&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SynchronousQueue&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractQueue&lt;E&gt;
-implements BlockingQueue&lt;E&gt;, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>public class</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Vector&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractList&lt;E&gt;
-implements List&lt;E&gt;, RandomAccess, Cloneable, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>public class</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> TreeSet&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractSet&lt;E&gt;
-implements NavigableSet&lt;E&gt;, Cloneable, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LinkedHashSet&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends HashSet&lt;E&gt;
-implements Set&lt;E&gt;, Cloneable, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <t>The Collections Framework</t>
-  </si>
-  <si>
-    <t>FIFO (first-in-first-out)</t>
-  </si>
-  <si>
-    <t>Interface Collection&lt;E&gt;</t>
-  </si>
-  <si>
-    <t>Interface Map&lt;K,V&gt;</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ArrayDeque&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractCollection&lt;E&gt;
-implements Deque&lt;E&gt;, Cloneable, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ArrayList&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractList&lt;E&gt;
-implements List&lt;E&gt;, RandomAccess, Cloneable, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ConcurrentLinkedQueue&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractQueue&lt;E&gt;
-implements Queue&lt;E&gt;, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ConcurrentSkipListSet&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractSet&lt;E&gt;
-implements NavigableSet&lt;E&gt;, Cloneable, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>public class</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CopyOnWriteArraySet&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractSet&lt;E&gt;
-implements Serializable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public class </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>HashSet&lt;E&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-extends AbstractSet&lt;E&gt;
-implements Set&lt;E&gt;, Cloneable, Serializable</t>
-    </r>
-  </si>
-  <si>
-    <t> last-in-first-out (LIFO) </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1007,6 +1031,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1017,12 +1047,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1331,7 +1355,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1345,7 +1369,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -1370,23 +1394,23 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="A2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -1397,7 +1421,7 @@
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1409,7 +1433,7 @@
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="5"/>
@@ -1421,7 +1445,7 @@
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1433,10 +1457,10 @@
     </row>
     <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1447,7 +1471,7 @@
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="6"/>
@@ -1459,7 +1483,7 @@
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
@@ -1471,7 +1495,7 @@
     </row>
     <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1483,7 +1507,7 @@
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1495,7 +1519,7 @@
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1507,7 +1531,7 @@
     </row>
     <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1519,10 +1543,10 @@
     </row>
     <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1533,7 +1557,7 @@
     </row>
     <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1545,7 +1569,7 @@
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1557,10 +1581,10 @@
     </row>
     <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1571,7 +1595,7 @@
     </row>
     <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
@@ -1583,7 +1607,7 @@
     </row>
     <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -1595,10 +1619,10 @@
     </row>
     <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>32</v>
+        <v>16</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1609,10 +1633,10 @@
     </row>
     <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1623,7 +1647,7 @@
     </row>
     <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
@@ -1635,7 +1659,7 @@
     </row>
     <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
@@ -1646,16 +1670,16 @@
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="13"/>
+      <c r="A24" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>

</xml_diff>